<commit_message>
compute load stats (standard deviation, period) for each element
</commit_message>
<xml_diff>
--- a/sofs/load_case_data.xlsx
+++ b/sofs/load_case_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/jan079_csiro_au/Documents/SOTS/SOTS-2025/SOFS-14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan079\GitHub\sots-cable-model\sofs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{C779C5D6-6309-480F-9E9A-57BFEE77C074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{038FA2BF-BA38-428C-922E-DB93F6B93C8D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4E930C-77D9-43D8-A4DA-5507C0EAD228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="2610" windowWidth="22920" windowHeight="17865" xr2:uid="{1C486731-3BF1-4942-A69C-5723B0554CEC}"/>
+    <workbookView xWindow="15480" yWindow="1845" windowWidth="22920" windowHeight="17865" xr2:uid="{1C486731-3BF1-4942-A69C-5723B0554CEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>10.5</v>
+        <v>9.6</v>
       </c>
       <c r="C11">
         <v>12.3</v>
@@ -719,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>11.4</v>
+        <v>10.5</v>
       </c>
       <c r="C12">
         <v>13.1</v>
@@ -739,7 +739,7 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>12.3</v>
+        <v>11.4</v>
       </c>
       <c r="C13">
         <v>13.9</v>
@@ -759,7 +759,7 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>13.2</v>
+        <v>12.3</v>
       </c>
       <c r="C14">
         <v>14.7</v>
@@ -779,7 +779,7 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>14.2</v>
+        <v>13.2</v>
       </c>
       <c r="C15">
         <v>15.5</v>
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>15.09</v>
+        <v>14.2</v>
       </c>
       <c r="C16">
         <v>16.3</v>
@@ -819,7 +819,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>15.09</v>
       </c>
       <c r="C17">
         <v>17.100000000000001</v>
@@ -839,7 +839,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>16.899999999999999</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>17.899999999999999</v>

</xml_diff>

<commit_message>
work on python processor to fatigue life
</commit_message>
<xml_diff>
--- a/sofs/load_case_data.xlsx
+++ b/sofs/load_case_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan079\GitHub\sots-cable-model\sofs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/GitHub/sots-cable-model/sofs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4E930C-77D9-43D8-A4DA-5507C0EAD228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609353C-9356-3447-831E-59AB05DFD590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="1845" windowWidth="22920" windowHeight="17865" xr2:uid="{1C486731-3BF1-4942-A69C-5723B0554CEC}"/>
+    <workbookView xWindow="15480" yWindow="1840" windowWidth="22920" windowHeight="17860" xr2:uid="{1C486731-3BF1-4942-A69C-5723B0554CEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>SWH</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>n17</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -489,34 +489,34 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1.4</v>
@@ -534,9 +534,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2.2999999999999998</v>
@@ -554,9 +554,9 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>3.2</v>
@@ -574,9 +574,9 @@
         <v>5.22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>4.0999999999999996</v>
@@ -594,9 +594,9 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -614,9 +614,9 @@
         <v>23.57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>5.9</v>
@@ -634,9 +634,9 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>6.8</v>
@@ -654,9 +654,9 @@
         <v>14.83</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>7.8</v>
@@ -674,9 +674,9 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>8.6999999999999993</v>
@@ -694,9 +694,9 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>9.6</v>
@@ -714,9 +714,9 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>10.5</v>
@@ -734,9 +734,9 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>11.4</v>
@@ -754,9 +754,9 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>12.3</v>
@@ -774,9 +774,9 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>13.2</v>
@@ -794,9 +794,9 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>14.2</v>
@@ -814,9 +814,9 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>15.09</v>
@@ -834,9 +834,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -854,9 +854,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19">
         <v>16.899999999999999</v>

</xml_diff>